<commit_message>
Test + adjust w template files
</commit_message>
<xml_diff>
--- a/conInfo/contrastInfo_basic.xlsx
+++ b/conInfo/contrastInfo_basic.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32040" yWindow="-1680" windowWidth="19840" windowHeight="14880" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="32040" yWindow="-1680" windowWidth="19840" windowHeight="14880" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="namesAndWeights" sheetId="1" r:id="rId1"/>
     <sheet name="condsRemoved" sheetId="4" r:id="rId2"/>
-    <sheet name="contrastWeights.txt" sheetId="2" r:id="rId3"/>
-    <sheet name="contrastNames.txt" sheetId="3" r:id="rId4"/>
+    <sheet name="contrastWeights_basic.txt" sheetId="2" r:id="rId3"/>
+    <sheet name="contrastNames_basic.txt" sheetId="3" r:id="rId4"/>
+    <sheet name="condsRemoved_basic.txt" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -209,8 +210,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -306,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -352,6 +355,7 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -397,6 +401,7 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2258,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4057,7 +4062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection sqref="A1:T23"/>
     </sheetView>
   </sheetViews>
@@ -5503,8 +5508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C23"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5648,4 +5653,1636 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:T26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+      <c r="R1">
+        <v>0</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add scaling for each side of the contrast, scaling by pos + neg sums
</commit_message>
<xml_diff>
--- a/conInfo/contrastInfo_basic.xlsx
+++ b/conInfo/contrastInfo_basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32040" yWindow="-1680" windowWidth="19840" windowHeight="14880" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="38440" yWindow="-1680" windowWidth="19840" windowHeight="14880" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="namesAndWeights" sheetId="1" r:id="rId1"/>
@@ -5659,8 +5659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>